<commit_message>
Fix activation of H2 Import
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SUP_H2Imp-On.xlsx
+++ b/SuppXLS/Scen_SUP_H2Imp-On.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2121FA-E98D-445E-986A-4E000FA2A937}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B65C4C-4E61-4B84-9459-9503A4517261}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="2985" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -1665,7 +1665,7 @@
   <dimension ref="B4:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1726,14 +1726,14 @@
         <v>68</v>
       </c>
       <c r="E6">
-        <v>2020</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G6">
         <f>F6</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I6" t="s">
         <v>70</v>

</xml_diff>